<commit_message>
modifiche a indice e checklist, eliminazione di pdf non più utili, come da richiesta
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="92">
   <si>
     <t xml:space="preserve">NOME FORNITORE:</t>
   </si>
@@ -220,15 +220,6 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:56:31Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b8780c91e24097c7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.d3ab21b14c9ec4ce46263ff1bf40f69430153b7208a01ab0c8d2ca45caf0ef63.a3855e979a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
@@ -299,7 +290,7 @@
     <t xml:space="preserve">L’utente viene avvertito del’errore  e viene pregato di riprovare successivamente – l’appllicativo manda una notifica agli sviluppatori in modo da risolvere il problema in breve tempo</t>
   </si>
   <si>
-    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token</t>
+    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token, com aggiuta di nuovi campi obbligatori</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
@@ -355,10 +346,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T11:06:40Z</t>
+    <t xml:space="preserve">Il dato è sanificato a priori</t>
   </si>
   <si>
-    <t xml:space="preserve">1aa975725e2f67d9</t>
+    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token non retrocompatibili</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_LDO_TIMEOUT</t>
@@ -379,15 +370,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 5" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:56:46Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f16ab0d01481f6aa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.fe3dd28aee3f03f22594b5f30f3e20ba12b44d92ba2472efb8e9fedee20148b9.cb5fa87ba9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">Viene controllato a priori che il dato esista</t>
   </si>
   <si>
@@ -402,33 +384,12 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 6" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:56:52Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">f55297466a1f27a0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.e09a04f79fb499fd0f90ba7b320d46e7f8c2049d754c447f7dde73afade1793c.2f4943d19f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il dato è sanificato a priori</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT7_KO</t>
   </si>
   <si>
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 7" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-02-06T08:56:57Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2249f92744cd1f50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.6ac8dd321b6144a28b9bbf21acff867729141989105991d1ca0f13ab824cd3cb.298e693f20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Al momento non abbiamo questa gestione nell’applicativo</t>
@@ -442,15 +403,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 8" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:57:30Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">feb47e81e75ca4c7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.e40072f20f12e689e6114d8da2b7311e06e2971b3001a6f56b8b363cc1dae391.0dffdd785f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validazione a priori dei dati anagrafici, ed eventuali indirizzi incompleti non vengono inseriti (ma il resto dell’anagrafica sì)</t>
   </si>
   <si>
@@ -460,15 +412,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 9" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-02-06T08:57:42Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14296e64251932a4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.82f10e5f6d47288d3eee7349aa21398ae9d9324324c96d7aa8d3bb1be61ae5f4.5fc8c7ee29^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Il software non tratta anagrafiche incomplete</t>
@@ -482,15 +425,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 10" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:57:47Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a84f3c8fa58bfc93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a2a83f3f28f5eadcdaba16c47f26eff6a4731e439241ccfc06f8869088677b76.56aa3bb260^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">Validazione del dato a livello del software</t>
   </si>
   <si>
@@ -500,15 +434,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation"al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 11" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-02-06T08:57:53Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dabeb75fa19b65a3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.019c6f224c4c883184c9fa292ab0df05b5849000709d0acd9f74ce731e89099f.c0642f1ace^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Validazione della presenza del dato a livello del software</t>
@@ -522,30 +447,12 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 12" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:57:58Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30066fa74a220436</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.82552d9bd9d5d64ed4a9be6e8ada0c647d41c78c01ec7b14799d81f0ad1523d2.a2708ba609^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT13_KO</t>
   </si>
   <si>
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-02-06T08:58:04Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a564fde46f506b4c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.cd14393cb10ae76521b58e6bb47f60f3123a99dbb38d5b8d2c96a4a67ef5defb.10757a8d22^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">Al momento abbiamo solo la gestione testuale dell’anamnesi</t>
@@ -559,15 +466,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 14" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:58:09Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cf246414f5252ef4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.1a13fc65323fedbd38bbb28ce338e814b23d3facdae1baeaab2ad18cd5ce8eb3.283c0bb76c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">Al momento abbiamo solo la gestione testuale del dato</t>
   </si>
   <si>
@@ -579,15 +477,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 15" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:58:15Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">807f4215c4b311c1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.4a2aa19ca36203bfec8669637167f3186787097d9d5559b10005e6ab27c447df.037acb1226^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t xml:space="preserve">Al momento abbiamo solo la gestione testuale del motivo del ricovero</t>
   </si>
   <si>
@@ -597,15 +486,6 @@
     <t xml:space="preserve">
 Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori terminologici sui Dati (status code 400), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway.
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 16" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-02-06T08:58:21Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3b87b2ac4633b8b4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.a0ff6f56a5f687e1e00dc7bde895901312a03d0c1c6e70a852122d4d605bafdd.37ccedeeca^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -977,7 +857,7 @@
       <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -1301,27 +1181,17 @@
       <c r="E13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="18"/>
       <c r="K13" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="L13" s="18" t="s">
-        <v>29</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L13" s="18"/>
       <c r="M13" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N13" s="19"/>
       <c r="O13" s="20"/>
@@ -1337,34 +1207,36 @@
         <v>21</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="H14" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="K14" s="18"/>
+      <c r="K14" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="L14" s="18"/>
       <c r="M14" s="18"/>
       <c r="N14" s="19" t="s">
         <v>28</v>
       </c>
       <c r="O14" s="22" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,34 +1250,28 @@
         <v>21</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="18"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
+      <c r="M15" s="18" t="s">
+        <v>53</v>
+      </c>
       <c r="N15" s="19" t="s">
         <v>28</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,19 +1285,21 @@
         <v>21</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
       <c r="J16" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="K16" s="18"/>
+        <v>57</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
       <c r="N16" s="19" t="s">
@@ -1450,36 +1318,28 @@
         <v>21</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>65</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="18"/>
       <c r="K17" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L17" s="18"/>
       <c r="M17" s="18" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="N17" s="19" t="s">
         <v>28</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1493,30 +1353,22 @@
         <v>21</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>72</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="18"/>
       <c r="K18" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L18" s="18"/>
       <c r="M18" s="18" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="N18" s="19" t="s">
         <v>28</v>
@@ -1534,30 +1386,22 @@
         <v>21</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>78</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="18"/>
       <c r="K19" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L19" s="18"/>
       <c r="M19" s="18" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="N19" s="19" t="s">
         <v>28</v>
@@ -1575,30 +1419,22 @@
         <v>21</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H20" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>84</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
       <c r="J20" s="18"/>
       <c r="K20" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L20" s="18"/>
       <c r="M20" s="18" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="N20" s="19" t="s">
         <v>28</v>
@@ -1616,30 +1452,22 @@
         <v>21</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>90</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
       <c r="J21" s="18"/>
       <c r="K21" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L21" s="18"/>
       <c r="M21" s="18" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="N21" s="19" t="s">
         <v>28</v>
@@ -1657,30 +1485,22 @@
         <v>21</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>96</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="18"/>
       <c r="K22" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L22" s="18"/>
       <c r="M22" s="18" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="N22" s="19" t="s">
         <v>28</v>
@@ -1698,30 +1518,22 @@
         <v>21</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="I23" s="17" t="s">
-        <v>102</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
       <c r="J23" s="18"/>
       <c r="K23" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L23" s="18"/>
       <c r="M23" s="18" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="N23" s="19" t="s">
         <v>28</v>
@@ -1739,30 +1551,22 @@
         <v>21</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>108</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="18"/>
       <c r="K24" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L24" s="18"/>
       <c r="M24" s="18" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="N24" s="19" t="s">
         <v>28</v>
@@ -1780,30 +1584,22 @@
         <v>21</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>109</v>
+        <v>81</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>113</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="18"/>
       <c r="K25" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L25" s="18"/>
       <c r="M25" s="18" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="N25" s="19" t="s">
         <v>28</v>
@@ -1821,30 +1617,22 @@
         <v>21</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F26" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="I26" s="17" t="s">
-        <v>119</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="18"/>
       <c r="K26" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L26" s="18"/>
       <c r="M26" s="18" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="N26" s="19" t="s">
         <v>28</v>
@@ -1862,30 +1650,22 @@
         <v>21</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G27" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="I27" s="17" t="s">
-        <v>125</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="18"/>
       <c r="K27" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L27" s="18"/>
       <c r="M27" s="18" t="s">
-        <v>126</v>
+        <v>89</v>
       </c>
       <c r="N27" s="19" t="s">
         <v>28</v>
@@ -1903,30 +1683,22 @@
         <v>21</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>127</v>
+        <v>90</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="H28" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>131</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="L28" s="18"/>
       <c r="M28" s="18" t="s">
-        <v>120</v>
+        <v>86</v>
       </c>
       <c r="N28" s="19" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
fix file CDA, aggiunti PDF segnati
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
@@ -160,16 +160,16 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">06/02/2023</t>
+    <t xml:space="preserve">20/02/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T10:58:01Z</t>
+    <t xml:space="preserve">2023-02-20T03:08:58Z</t>
   </si>
   <si>
-    <t xml:space="preserve">42ca09e04c2fb81c</t>
+    <t xml:space="preserve">a3836b1e2ceba814</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.85cdde3e4bb5b1d83cf22e9157d2bf7f32e55a9ad1e3343e76513e83a0345e87.877921c7ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.d28e3aa1463221ed2bf8a5d56997a019e2cff0165ab40a65c8ea0e8bb050d2e4.dc74965ed7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -186,13 +186,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:56:21Z</t>
+    <t xml:space="preserve">2023-02-20T03:09:13Z</t>
   </si>
   <si>
-    <t xml:space="preserve">ac5cc3693be914d4</t>
+    <t xml:space="preserve">e4dd006aee4f5485</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.4d3ebc72e5a2bd190a0158b07b19ba882487f121e19ea708f70fcb6a8d6884c2.9a091975a8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.f458ca3bdeb07d7940d52a08e32cb7037b61302cadfbe08538e8155fb45f1376.5641cf5194^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -203,13 +203,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T08:56:26Z</t>
+    <t xml:space="preserve">2023-02-20T03:09:27Z</t>
   </si>
   <si>
-    <t xml:space="preserve">1b6b417e1be7577a</t>
+    <t xml:space="preserve">d1b892901ad0688d</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.120.4.4.933abdb3ed33043f09642c988875b483e21a6dcae7fb19a3a92967de3b3bd6f4.3027c17c37^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.bbef8984860320c53906d495632da2c7cd685c7de57b875a697f14d7708a3985.2667f3d4b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">Il nostro software non gestisce tutti i campi possibili della LDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token, com aggiuta di nuovi campi obbligatori</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
@@ -278,10 +281,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-06T10:58:15Z</t>
+    <t xml:space="preserve">2023-02-20T03:09:37Z</t>
   </si>
   <si>
-    <t xml:space="preserve">dc1ba4ce4e135ef5</t>
+    <t xml:space="preserve">76d98f275c8fe8e8</t>
   </si>
   <si>
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
@@ -290,7 +293,10 @@
     <t xml:space="preserve">L’utente viene avvertito del’errore  e viene pregato di riprovare successivamente – l’appllicativo manda una notifica agli sviluppatori in modo da risolvere il problema in breve tempo</t>
   </si>
   <si>
-    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token, com aggiuta di nuovi campi obbligatori</t>
+    <t xml:space="preserve">FAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token non retrocompatibili</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
@@ -349,9 +355,6 @@
     <t xml:space="preserve">Il dato è sanificato a priori</t>
   </si>
   <si>
-    <t xml:space="preserve">L’errore si può verificare solo in caso di cambio di specifiche di generazione di token non retrocompatibili</t>
-  </si>
-  <si>
     <t xml:space="preserve">VALIDAZIONE_LDO_TIMEOUT</t>
   </si>
   <si>
@@ -359,7 +362,7 @@
 Per questo caso di test è richiesta la  sola descrizione del comportamento a fronte di un timeout, da inserire nella colonna "J" nominata come "GESTIONE ERRORE".</t>
   </si>
   <si>
-    <t xml:space="preserve">L’utente viene avvertito del timeout e viene pregato di riprovare successivamente</t>
+    <t xml:space="preserve">L’errore non è comunque quello richiesto, vedere https://github.com/ministero-salute/it-fse-support/issues/44</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT5_KO</t>
@@ -371,9 +374,6 @@
   </si>
   <si>
     <t xml:space="preserve">Viene controllato a priori che il dato esista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L’errore non è comunque quello richiesto, vedere https://github.com/ministero-salute/it-fse-support/issues/44</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT6_KO</t>
@@ -497,7 +497,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -535,6 +535,13 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -649,7 +656,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -698,6 +705,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -726,6 +737,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -734,12 +749,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -854,21 +873,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="O16" activeCellId="0" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="39.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="33.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="62.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="27.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="33.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="36.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="16" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -1001,7 +1019,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1050,7 @@
       <c r="J9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" s="12" t="s">
         <v>15</v>
       </c>
       <c r="L9" s="11" t="s">
@@ -1041,7 +1059,7 @@
       <c r="M9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="12" t="s">
+      <c r="N9" s="13" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="11" t="s">
@@ -1049,661 +1067,661 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="n">
+      <c r="A10" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18" t="s">
+      <c r="J10" s="19"/>
+      <c r="K10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19"/>
-      <c r="O10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="n">
+      <c r="A11" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="18"/>
-      <c r="K11" s="18" t="s">
+      <c r="J11" s="19"/>
+      <c r="K11" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="18" t="s">
+      <c r="L11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="18"/>
-      <c r="N11" s="19"/>
-      <c r="O11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="n">
+      <c r="A12" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18" t="s">
+      <c r="J12" s="19"/>
+      <c r="K12" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="22"/>
     </row>
     <row r="13" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="n">
+      <c r="A13" s="14" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18" t="s">
+      <c r="F13" s="17"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="18"/>
-      <c r="M13" s="18" t="s">
+      <c r="L13" s="19"/>
+      <c r="M13" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="19"/>
-      <c r="O13" s="20"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="23" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="n">
+      <c r="A14" s="14" t="n">
         <v>29</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="21" t="s">
+      <c r="D14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="E14" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="17" t="s">
+      <c r="G14" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="H14" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="I14" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="18" t="s">
+      <c r="J14" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="18"/>
-      <c r="M14" s="18"/>
-      <c r="N14" s="19" t="s">
+      <c r="L14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="M14" s="20"/>
+      <c r="N14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="22" t="s">
-        <v>50</v>
+      <c r="O14" s="23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="n">
+      <c r="A15" s="14" t="n">
         <v>37</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="18" t="s">
+      <c r="D15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="17"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="N15" s="19" t="s">
+      <c r="L15" s="19"/>
+      <c r="M15" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="N15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="22" t="s">
-        <v>54</v>
-      </c>
+      <c r="O15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="n">
+      <c r="A16" s="14" t="n">
         <v>45</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" s="19"/>
+      <c r="M16" s="20"/>
+      <c r="N16" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="n">
+        <v>63</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="25"/>
+    </row>
+    <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="n">
+        <v>64</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" s="19"/>
+      <c r="M18" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="18" t="s">
+      <c r="N18" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="18"/>
-      <c r="M16" s="18"/>
-      <c r="N16" s="19" t="s">
+      <c r="O18" s="25"/>
+    </row>
+    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="n">
+        <v>65</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" s="19"/>
+      <c r="M19" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="N19" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="20"/>
-    </row>
-    <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="n">
-        <v>63</v>
-      </c>
-      <c r="B17" s="14" t="s">
+      <c r="O19" s="25"/>
+    </row>
+    <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="n">
+        <v>66</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C20" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18" t="s">
+      <c r="D20" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="17"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="N17" s="19" t="s">
+      <c r="L20" s="19"/>
+      <c r="M20" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="N20" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="n">
-        <v>64</v>
-      </c>
-      <c r="B18" s="14" t="s">
+      <c r="O20" s="25"/>
+    </row>
+    <row r="21" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
+        <v>67</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18" t="s">
+      <c r="D21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="17"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="N18" s="19" t="s">
+      <c r="L21" s="19"/>
+      <c r="M21" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="N21" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="20"/>
-    </row>
-    <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="n">
-        <v>65</v>
-      </c>
-      <c r="B19" s="14" t="s">
+      <c r="O21" s="25"/>
+    </row>
+    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="n">
+        <v>68</v>
+      </c>
+      <c r="B22" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="18" t="s">
+      <c r="D22" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="N19" s="19" t="s">
+      <c r="L22" s="19"/>
+      <c r="M22" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="N22" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O19" s="20"/>
-    </row>
-    <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="n">
-        <v>66</v>
-      </c>
-      <c r="B20" s="14" t="s">
+      <c r="O22" s="25"/>
+    </row>
+    <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="n">
+        <v>69</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18" t="s">
+      <c r="D23" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F23" s="17"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="18"/>
-      <c r="M20" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="N20" s="19" t="s">
+      <c r="L23" s="19"/>
+      <c r="M23" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N23" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="20"/>
-    </row>
-    <row r="21" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="n">
-        <v>67</v>
-      </c>
-      <c r="B21" s="14" t="s">
+      <c r="O23" s="25"/>
+    </row>
+    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="n">
+        <v>70</v>
+      </c>
+      <c r="B24" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C24" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="15" t="s">
+      <c r="D24" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F24" s="17"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="N24" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="25"/>
+    </row>
+    <row r="25" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="n">
         <v>71</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18" t="s">
+      <c r="B25" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18" t="s">
+      <c r="L25" s="19"/>
+      <c r="M25" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="N25" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="n">
         <v>72</v>
       </c>
-      <c r="N21" s="19" t="s">
+      <c r="B26" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="17"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L26" s="19"/>
+      <c r="M26" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="N26" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O21" s="20"/>
-    </row>
-    <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="n">
-        <v>68</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="O26" s="25"/>
+    </row>
+    <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="n">
+        <v>73</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="15" t="s">
+      <c r="D27" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L27" s="19"/>
+      <c r="M27" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="N27" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O27" s="25"/>
+    </row>
+    <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="n">
         <v>74</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18" t="s">
+      <c r="B28" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" s="17"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="N22" s="19" t="s">
+      <c r="L28" s="19"/>
+      <c r="M28" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="N28" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="O22" s="20"/>
-    </row>
-    <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="n">
-        <v>69</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="N23" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="20"/>
-    </row>
-    <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="n">
-        <v>70</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O24" s="20"/>
-    </row>
-    <row r="25" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="n">
-        <v>71</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="N25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O25" s="20"/>
-    </row>
-    <row r="26" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="n">
-        <v>72</v>
-      </c>
-      <c r="B26" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="N26" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O26" s="20"/>
-    </row>
-    <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="n">
-        <v>73</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="N27" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O27" s="20"/>
-    </row>
-    <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="n">
-        <v>74</v>
-      </c>
-      <c r="B28" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="L28" s="18"/>
-      <c r="M28" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="N28" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="O28" s="20"/>
+      <c r="O28" s="25"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F29" s="1"/>
@@ -11857,7 +11875,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="O17" r:id="rId2" display="L’errore non è comunque quello richiesto, vedere https://github.com/ministero-salute/it-fse-support/issues/44"/>
+    <hyperlink ref="O16" r:id="rId2" display="L’errore non è comunque quello richiesto, vedere https://github.com/ministero-salute/it-fse-support/issues/44"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
nuovi risultati dopo ulteriore correzione CDA e nuovo invio al GTW
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
@@ -160,16 +160,16 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">20/02/2023</t>
+    <t xml:space="preserve">23/02/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-20T03:08:58Z</t>
+    <t xml:space="preserve">2023-02-23T08:46:44Z</t>
   </si>
   <si>
-    <t xml:space="preserve">a3836b1e2ceba814</t>
+    <t xml:space="preserve">95100c0d717c867d</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.d28e3aa1463221ed2bf8a5d56997a019e2cff0165ab40a65c8ea0e8bb050d2e4.dc74965ed7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.d2bb9156f5cd358eb44d7046ff96bf4623c537d0cc904bf8f21f9884daf1dd4c.4b24c462b1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -186,13 +186,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-20T03:09:13Z</t>
+    <t xml:space="preserve">2023-02-23T08:46:57Z</t>
   </si>
   <si>
-    <t xml:space="preserve">e4dd006aee4f5485</t>
+    <t xml:space="preserve">ebc09f98c0e4cd29</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.f458ca3bdeb07d7940d52a08e32cb7037b61302cadfbe08538e8155fb45f1376.5641cf5194^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.839786fc8e14e7a459b547d4054b513f0fefd73b884834376eb139f9473ca806.5a087bf33b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT3</t>
@@ -203,13 +203,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-20T03:09:27Z</t>
+    <t xml:space="preserve">2023-02-23T08:47:04Z</t>
   </si>
   <si>
-    <t xml:space="preserve">d1b892901ad0688d</t>
+    <t xml:space="preserve">5fa4e6819754065e</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.bbef8984860320c53906d495632da2c7cd685c7de57b875a697f14d7708a3985.2667f3d4b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.110.4.4.37a379c50a941d0c8ac7cdb73b9d11f629f320e50f254b681ed8797b2a55a353.491c29cfb2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT4</t>
@@ -281,10 +281,10 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">2023-02-20T03:09:37Z</t>
+    <t xml:space="preserve">2023-02-23T08:47:12Z</t>
   </si>
   <si>
-    <t xml:space="preserve">76d98f275c8fe8e8</t>
+    <t xml:space="preserve">6f1fab58014ba6e2</t>
   </si>
   <si>
     <t xml:space="preserve">UNKNOWN_WORKFLOW_ID</t>
@@ -497,7 +497,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -535,13 +535,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -656,7 +649,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -705,10 +698,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
@@ -737,10 +726,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -753,12 +738,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -873,10 +862,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="O16" activeCellId="0" sqref="O16"/>
+      <selection pane="bottomRight" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -884,9 +873,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="104.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="33.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="36.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="31.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="16" style="0" width="8.71"/>
   </cols>
   <sheetData>
@@ -1050,7 +1039,7 @@
       <c r="J9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="11" t="s">
         <v>15</v>
       </c>
       <c r="L9" s="11" t="s">
@@ -1059,7 +1048,7 @@
       <c r="M9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="N9" s="13" t="s">
+      <c r="N9" s="12" t="s">
         <v>18</v>
       </c>
       <c r="O9" s="11" t="s">
@@ -1067,661 +1056,661 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="14" t="n">
+      <c r="A10" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19" t="s">
+      <c r="J10" s="18"/>
+      <c r="K10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M10" s="20"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="22"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="n">
+      <c r="A11" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19" t="s">
+      <c r="J11" s="18"/>
+      <c r="K11" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L11" s="19" t="s">
+      <c r="L11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="20"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="22"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="20"/>
     </row>
     <row r="12" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="n">
+      <c r="A12" s="13" t="n">
         <v>8</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="18" t="s">
+      <c r="I12" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19" t="s">
+      <c r="J12" s="18"/>
+      <c r="K12" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="19" t="s">
+      <c r="L12" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="20"/>
-      <c r="N12" s="21"/>
-      <c r="O12" s="22"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="20"/>
     </row>
     <row r="13" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="13" t="n">
         <v>9</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="18"/>
+      <c r="K13" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L13" s="19"/>
-      <c r="M13" s="20" t="s">
+      <c r="L13" s="18"/>
+      <c r="M13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="N13" s="21"/>
-      <c r="O13" s="23" t="s">
+      <c r="N13" s="19"/>
+      <c r="O13" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="n">
+      <c r="A14" s="13" t="n">
         <v>29</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="K14" s="19" t="s">
+      <c r="K14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="19" t="s">
+      <c r="L14" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="M14" s="20"/>
-      <c r="N14" s="21" t="s">
+      <c r="M14" s="18"/>
+      <c r="N14" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="O14" s="21" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="n">
+      <c r="A15" s="13" t="n">
         <v>37</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19" t="s">
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="19"/>
-      <c r="M15" s="20" t="s">
+      <c r="L15" s="18"/>
+      <c r="M15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N15" s="21" t="s">
+      <c r="N15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O15" s="22"/>
+      <c r="O15" s="20"/>
     </row>
     <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="n">
+      <c r="A16" s="13" t="n">
         <v>45</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="21" t="s">
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="21" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="n">
+      <c r="A17" s="13" t="n">
         <v>63</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19" t="s">
+      <c r="F17" s="23"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="20" t="s">
+      <c r="L17" s="18"/>
+      <c r="M17" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="N17" s="21" t="s">
+      <c r="N17" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="25"/>
+      <c r="O17" s="20"/>
     </row>
     <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="n">
+      <c r="A18" s="13" t="n">
         <v>64</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19" t="s">
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="20" t="s">
+      <c r="L18" s="18"/>
+      <c r="M18" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N18" s="21" t="s">
+      <c r="N18" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O18" s="25"/>
+      <c r="O18" s="20"/>
     </row>
     <row r="19" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="n">
+      <c r="A19" s="13" t="n">
         <v>65</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19" t="s">
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L19" s="19"/>
-      <c r="M19" s="20" t="s">
+      <c r="L19" s="18"/>
+      <c r="M19" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="N19" s="21" t="s">
+      <c r="N19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O19" s="25"/>
+      <c r="O19" s="20"/>
     </row>
     <row r="20" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="n">
+      <c r="A20" s="13" t="n">
         <v>66</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19" t="s">
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="20" t="s">
+      <c r="L20" s="18"/>
+      <c r="M20" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="N20" s="21" t="s">
+      <c r="N20" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O20" s="25"/>
+      <c r="O20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="14" t="n">
+      <c r="A21" s="13" t="n">
         <v>67</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="19"/>
-      <c r="K21" s="19" t="s">
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="20" t="s">
+      <c r="L21" s="18"/>
+      <c r="M21" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="N21" s="21" t="s">
+      <c r="N21" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O21" s="25"/>
+      <c r="O21" s="20"/>
     </row>
     <row r="22" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="14" t="n">
+      <c r="A22" s="13" t="n">
         <v>68</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="19"/>
-      <c r="K22" s="19" t="s">
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="20" t="s">
+      <c r="L22" s="18"/>
+      <c r="M22" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="N22" s="21" t="s">
+      <c r="N22" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O22" s="25"/>
+      <c r="O22" s="20"/>
     </row>
     <row r="23" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="n">
+      <c r="A23" s="13" t="n">
         <v>69</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19" t="s">
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="20" t="s">
+      <c r="L23" s="18"/>
+      <c r="M23" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N23" s="21" t="s">
+      <c r="N23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O23" s="25"/>
+      <c r="O23" s="20"/>
     </row>
     <row r="24" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="n">
+      <c r="A24" s="13" t="n">
         <v>70</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="17"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19" t="s">
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L24" s="19"/>
-      <c r="M24" s="20" t="s">
+      <c r="L24" s="18"/>
+      <c r="M24" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="N24" s="21" t="s">
+      <c r="N24" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O24" s="25"/>
+      <c r="O24" s="20"/>
     </row>
     <row r="25" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="n">
+      <c r="A25" s="13" t="n">
         <v>71</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19" t="s">
+      <c r="F25" s="23"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="20" t="s">
+      <c r="L25" s="18"/>
+      <c r="M25" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="N25" s="21" t="s">
+      <c r="N25" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O25" s="25"/>
+      <c r="O25" s="20"/>
     </row>
     <row r="26" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="n">
+      <c r="A26" s="13" t="n">
         <v>72</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="F26" s="17"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19" t="s">
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L26" s="19"/>
-      <c r="M26" s="20" t="s">
+      <c r="L26" s="18"/>
+      <c r="M26" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="N26" s="21" t="s">
+      <c r="N26" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="25"/>
+      <c r="O26" s="20"/>
     </row>
     <row r="27" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="n">
+      <c r="A27" s="13" t="n">
         <v>73</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19" t="s">
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="19"/>
-      <c r="M27" s="20" t="s">
+      <c r="L27" s="18"/>
+      <c r="M27" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="N27" s="21" t="s">
+      <c r="N27" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O27" s="25"/>
+      <c r="O27" s="20"/>
     </row>
     <row r="28" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="n">
+      <c r="A28" s="13" t="n">
         <v>74</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="17"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19" t="s">
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="L28" s="19"/>
-      <c r="M28" s="20" t="s">
+      <c r="L28" s="18"/>
+      <c r="M28" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="N28" s="21" t="s">
+      <c r="N28" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="O28" s="25"/>
+      <c r="O28" s="20"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F29" s="1"/>

</xml_diff>

<commit_message>
compilazione campi mancanti report-checklist.xlsx
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
+++ b/GATEWAY/A1#111GRUPPOSID00/SID_SRL/SICO/V2023/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="207">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -524,6 +524,9 @@
   <si>
     <t xml:space="preserve">Per questo caso di test è richiesta la sola descrizione del comportamento a fronte di un timeout, da inserire nelle colonne relative a:
 "ERRORE BLOCCANTE (SI/NO)", "ERRORE VISIBILE A UTENTE (SI/NO)", "MESSAGGIO DI ERRORE", "GESTITO IN BACKOFFICE (SI/NO)", " PRESENTE CODA DI RETRY AUTOMATICA PER L'INVIO DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)",  "INVIO MANUALE DEL DOCUMENTO AL FSE A SEGUITO DELLA RISOLUZIONE DELL'ERRORE (SI/NO)", "GESTIONE ERRORE".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il Gateway di validazione non è raggiungibile</t>
   </si>
   <si>
     <t xml:space="preserve">L'applicativo SICO invia tramite log ed email una notifica all'assistenza di SID srl. Risolta la problematica, l'applicativo rigenera il token e all'utente viene notificato di firmare il documento, completata la validazione.</t>
@@ -1747,7 +1750,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1761,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2911,11 +2914,11 @@
   <dimension ref="A1:W640"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3200,7 +3203,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="88.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="26" t="n">
         <v>6</v>
       </c>
@@ -3247,7 +3250,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="88.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="26" t="n">
         <v>7</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="88.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="n">
         <v>8</v>
       </c>
@@ -3335,7 +3338,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="88.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="26" t="n">
         <v>9</v>
       </c>
@@ -3376,7 +3379,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="26" t="n">
         <v>29</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>71</v>
       </c>
       <c r="P14" s="31" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="Q14" s="31" t="s">
         <v>53</v>
@@ -3439,7 +3442,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="26" t="n">
         <v>32</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="26" t="n">
         <v>37</v>
       </c>
@@ -3521,7 +3524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="26" t="n">
         <v>40</v>
       </c>
@@ -3562,7 +3565,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="88.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="26" t="n">
         <v>45</v>
       </c>
@@ -3582,19 +3585,31 @@
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
-      <c r="J18" s="32"/>
+      <c r="J18" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
+      <c r="M18" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="R18" s="31" t="s">
         <v>53</v>
       </c>
       <c r="S18" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="T18" s="32"/>
       <c r="U18" s="38" t="s">
@@ -3616,7 +3631,7 @@
         <v>75</v>
       </c>
       <c r="D19" s="27" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E19" s="28" t="s">
         <v>82</v>
@@ -3625,19 +3640,31 @@
       <c r="G19" s="35"/>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
-      <c r="J19" s="32"/>
+      <c r="J19" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="32"/>
+      <c r="M19" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="P19" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q19" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="R19" s="31" t="s">
         <v>53</v>
       </c>
       <c r="S19" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="T19" s="32"/>
       <c r="U19" s="38" t="s">
@@ -3648,7 +3675,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="26" t="n">
         <v>63</v>
       </c>
@@ -3659,10 +3686,10 @@
         <v>47</v>
       </c>
       <c r="D20" s="27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" s="29"/>
       <c r="G20" s="35"/>
@@ -3689,7 +3716,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="26" t="n">
         <v>64</v>
       </c>
@@ -3700,10 +3727,10 @@
         <v>47</v>
       </c>
       <c r="D21" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E21" s="28" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F21" s="29"/>
       <c r="G21" s="35"/>
@@ -3713,7 +3740,7 @@
         <v>62</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L21" s="32"/>
       <c r="M21" s="32"/>
@@ -3730,7 +3757,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="n">
         <v>65</v>
       </c>
@@ -3741,10 +3768,10 @@
         <v>47</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="35"/>
@@ -3771,7 +3798,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="26" t="n">
         <v>66</v>
       </c>
@@ -3782,10 +3809,10 @@
         <v>47</v>
       </c>
       <c r="D23" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F23" s="29"/>
       <c r="G23" s="35"/>
@@ -3795,7 +3822,7 @@
         <v>62</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L23" s="32"/>
       <c r="M23" s="32"/>
@@ -3812,7 +3839,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="n">
         <v>67</v>
       </c>
@@ -3823,10 +3850,10 @@
         <v>47</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F24" s="29"/>
       <c r="G24" s="35"/>
@@ -3836,7 +3863,7 @@
         <v>62</v>
       </c>
       <c r="K24" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L24" s="32"/>
       <c r="M24" s="32"/>
@@ -3853,7 +3880,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="n">
         <v>68</v>
       </c>
@@ -3864,10 +3891,10 @@
         <v>47</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E25" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F25" s="29"/>
       <c r="G25" s="35"/>
@@ -3877,7 +3904,7 @@
         <v>62</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L25" s="32"/>
       <c r="M25" s="32"/>
@@ -3894,7 +3921,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="26" t="n">
         <v>69</v>
       </c>
@@ -3905,10 +3932,10 @@
         <v>47</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F26" s="29"/>
       <c r="G26" s="35"/>
@@ -3918,7 +3945,7 @@
         <v>62</v>
       </c>
       <c r="K26" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L26" s="32"/>
       <c r="M26" s="32"/>
@@ -3935,7 +3962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="26" t="n">
         <v>70</v>
       </c>
@@ -3946,10 +3973,10 @@
         <v>47</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="35"/>
@@ -3959,7 +3986,7 @@
         <v>62</v>
       </c>
       <c r="K27" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L27" s="32"/>
       <c r="M27" s="32"/>
@@ -3976,7 +4003,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="26" t="n">
         <v>71</v>
       </c>
@@ -3987,10 +4014,10 @@
         <v>47</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F28" s="29"/>
       <c r="G28" s="35"/>
@@ -4017,7 +4044,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="26" t="n">
         <v>72</v>
       </c>
@@ -4028,10 +4055,10 @@
         <v>47</v>
       </c>
       <c r="D29" s="27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F29" s="29"/>
       <c r="G29" s="35"/>
@@ -4058,7 +4085,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="26" t="n">
         <v>73</v>
       </c>
@@ -4069,10 +4096,10 @@
         <v>47</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F30" s="29"/>
       <c r="G30" s="35"/>
@@ -4099,7 +4126,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="26" t="n">
         <v>74</v>
       </c>
@@ -4110,10 +4137,10 @@
         <v>47</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F31" s="29"/>
       <c r="G31" s="35"/>
@@ -4140,7 +4167,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="26" t="n">
         <v>147</v>
       </c>
@@ -4151,10 +4178,10 @@
         <v>75</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E32" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F32" s="29"/>
       <c r="G32" s="35"/>
@@ -4181,7 +4208,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="26" t="n">
         <v>148</v>
       </c>
@@ -4192,10 +4219,10 @@
         <v>75</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E33" s="28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F33" s="29"/>
       <c r="G33" s="35"/>
@@ -4222,7 +4249,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="26" t="n">
         <v>149</v>
       </c>
@@ -4233,10 +4260,10 @@
         <v>75</v>
       </c>
       <c r="D34" s="27" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E34" s="28" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="35"/>
@@ -4263,7 +4290,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="26" t="n">
         <v>150</v>
       </c>
@@ -4274,10 +4301,10 @@
         <v>75</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F35" s="29"/>
       <c r="G35" s="35"/>
@@ -4304,7 +4331,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="26" t="n">
         <v>151</v>
       </c>
@@ -4315,10 +4342,10 @@
         <v>75</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E36" s="28" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F36" s="29"/>
       <c r="G36" s="35"/>
@@ -4345,7 +4372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="26" t="n">
         <v>152</v>
       </c>
@@ -4356,10 +4383,10 @@
         <v>75</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E37" s="28" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F37" s="29"/>
       <c r="G37" s="35"/>
@@ -4369,7 +4396,7 @@
         <v>62</v>
       </c>
       <c r="K37" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L37" s="32"/>
       <c r="M37" s="32"/>
@@ -4386,7 +4413,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="26" t="n">
         <v>153</v>
       </c>
@@ -4397,10 +4424,10 @@
         <v>75</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="35"/>
@@ -4427,7 +4454,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="26" t="n">
         <v>154</v>
       </c>
@@ -4438,10 +4465,10 @@
         <v>75</v>
       </c>
       <c r="D39" s="27" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="35"/>
@@ -4451,7 +4478,7 @@
         <v>62</v>
       </c>
       <c r="K39" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L39" s="32"/>
       <c r="M39" s="32"/>
@@ -4468,7 +4495,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="26" t="n">
         <v>155</v>
       </c>
@@ -4479,10 +4506,10 @@
         <v>75</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F40" s="29"/>
       <c r="G40" s="35"/>
@@ -4492,7 +4519,7 @@
         <v>62</v>
       </c>
       <c r="K40" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L40" s="32"/>
       <c r="M40" s="32"/>
@@ -4509,7 +4536,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="26" t="n">
         <v>156</v>
       </c>
@@ -4520,10 +4547,10 @@
         <v>75</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E41" s="28" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F41" s="29"/>
       <c r="G41" s="35"/>
@@ -4533,7 +4560,7 @@
         <v>62</v>
       </c>
       <c r="K41" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="L41" s="32"/>
       <c r="M41" s="32"/>
@@ -4550,7 +4577,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="26" t="n">
         <v>157</v>
       </c>
@@ -4561,10 +4588,10 @@
         <v>75</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="35"/>
@@ -4591,7 +4618,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="26" t="n">
         <v>158</v>
       </c>
@@ -4602,10 +4629,10 @@
         <v>75</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E43" s="28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F43" s="29"/>
       <c r="G43" s="35"/>
@@ -4632,7 +4659,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="26" t="n">
         <v>159</v>
       </c>
@@ -4643,10 +4670,10 @@
         <v>75</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F44" s="29"/>
       <c r="G44" s="35"/>
@@ -4673,7 +4700,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="26" t="n">
         <v>160</v>
       </c>
@@ -4684,10 +4711,10 @@
         <v>75</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F45" s="29"/>
       <c r="G45" s="35"/>
@@ -4697,7 +4724,7 @@
         <v>62</v>
       </c>
       <c r="K45" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L45" s="32"/>
       <c r="M45" s="32"/>
@@ -4714,7 +4741,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="26" t="n">
         <v>161</v>
       </c>
@@ -4725,10 +4752,10 @@
         <v>75</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F46" s="29"/>
       <c r="G46" s="35"/>
@@ -4738,7 +4765,7 @@
         <v>62</v>
       </c>
       <c r="K46" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L46" s="32"/>
       <c r="M46" s="32"/>
@@ -4755,7 +4782,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="26" t="n">
         <v>162</v>
       </c>
@@ -4766,10 +4793,10 @@
         <v>75</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F47" s="29"/>
       <c r="G47" s="35"/>
@@ -4779,7 +4806,7 @@
         <v>62</v>
       </c>
       <c r="K47" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L47" s="32"/>
       <c r="M47" s="32"/>
@@ -4796,7 +4823,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="26" t="n">
         <v>163</v>
       </c>
@@ -4807,10 +4834,10 @@
         <v>75</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E48" s="28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F48" s="29"/>
       <c r="G48" s="35"/>
@@ -4820,7 +4847,7 @@
         <v>62</v>
       </c>
       <c r="K48" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="L48" s="32"/>
       <c r="M48" s="32"/>
@@ -4837,7 +4864,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="26" t="n">
         <v>164</v>
       </c>
@@ -4848,10 +4875,10 @@
         <v>75</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="35"/>
@@ -4878,7 +4905,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="26" t="n">
         <v>165</v>
       </c>
@@ -4889,10 +4916,10 @@
         <v>75</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E50" s="28" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F50" s="29"/>
       <c r="G50" s="35"/>
@@ -4919,7 +4946,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="26" t="n">
         <v>166</v>
       </c>
@@ -4930,10 +4957,10 @@
         <v>75</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E51" s="28" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="35"/>
@@ -4960,7 +4987,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="26" t="n">
         <v>167</v>
       </c>
@@ -4971,10 +4998,10 @@
         <v>75</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E52" s="28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="35"/>
@@ -5001,7 +5028,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="26" t="n">
         <v>168</v>
       </c>
@@ -5012,10 +5039,10 @@
         <v>75</v>
       </c>
       <c r="D53" s="27" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E53" s="28" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F53" s="29"/>
       <c r="G53" s="35"/>
@@ -5042,7 +5069,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="77.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="26" t="n">
         <v>169</v>
       </c>
@@ -5053,10 +5080,10 @@
         <v>75</v>
       </c>
       <c r="D54" s="27" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E54" s="28" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F54" s="29"/>
       <c r="G54" s="35"/>
@@ -5083,7 +5110,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="88.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="26" t="n">
         <v>369</v>
       </c>
@@ -5094,22 +5121,22 @@
         <v>47</v>
       </c>
       <c r="D55" s="27" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E55" s="28" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F55" s="29" t="n">
         <v>45568</v>
       </c>
       <c r="G55" s="30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H55" s="30" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="I55" s="30" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="J55" s="31" t="s">
         <v>53</v>
@@ -5130,7 +5157,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="99.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="26" t="n">
         <v>374</v>
       </c>
@@ -5141,22 +5168,22 @@
         <v>75</v>
       </c>
       <c r="D56" s="27" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E56" s="28" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F56" s="29" t="n">
         <v>45568</v>
       </c>
       <c r="G56" s="30" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I56" s="30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="J56" s="31" t="s">
         <v>53</v>
@@ -9820,7 +9847,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9830,7 +9857,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9840,22 +9867,22 @@
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -9895,36 +9922,36 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="40" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F1" s="41" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="G1" s="42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="43" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9932,69 +9959,69 @@
         <v>47</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D3" s="44" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="43" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C4" s="44" t="n">
         <v>446.447</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D5" s="44" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="43" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10002,55 +10029,55 @@
         <v>75</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D8" s="45" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="43" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B9" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B10" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="43" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B11" s="43" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -11043,7 +11070,7 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="46" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>53</v>
@@ -11051,7 +11078,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="46" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B3" s="46" t="s">
         <v>62</v>

</xml_diff>